<commit_message>
Minor changes to 'FPGA GPIO pin assignments.xlsx' (formatting only)
</commit_message>
<xml_diff>
--- a/FPGA GPIO pin assignments.xlsx
+++ b/FPGA GPIO pin assignments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="23955" windowHeight="12330"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19440" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="GPIO pins" sheetId="1" r:id="rId1"/>
@@ -919,18 +919,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" style="12" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="9" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="9" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="9" customWidth="1"/>
     <col min="8" max="8" width="16" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -991,71 +991,66 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="5">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="A3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="4">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="4">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>7</v>
@@ -1066,54 +1061,40 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="4">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="6">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>108</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>7</v>
+        <v>52</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="13"/>
+      <c r="J7" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1121,22 +1102,22 @@
         <v>98</v>
       </c>
       <c r="B8" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>7</v>
@@ -1147,19 +1128,19 @@
         <v>98</v>
       </c>
       <c r="B9" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>7</v>
@@ -1173,19 +1154,19 @@
         <v>98</v>
       </c>
       <c r="B10" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>7</v>
@@ -1199,19 +1180,19 @@
         <v>98</v>
       </c>
       <c r="B11" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>7</v>
@@ -1221,81 +1202,85 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="4">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="18">
+        <v>5</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="4">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="A13" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="18">
+        <v>6</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B14" s="4">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1303,25 +1288,25 @@
         <v>98</v>
       </c>
       <c r="B15" s="4">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1329,25 +1314,25 @@
         <v>98</v>
       </c>
       <c r="B16" s="4">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1355,93 +1340,79 @@
         <v>98</v>
       </c>
       <c r="B17" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H17" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="4">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18"/>
-      <c r="J18"/>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="4">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19"/>
-      <c r="J19"/>
+      <c r="A19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="5">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B20" s="4">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>4</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1449,19 +1420,25 @@
         <v>98</v>
       </c>
       <c r="B21" s="4">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>17</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1469,19 +1446,25 @@
         <v>98</v>
       </c>
       <c r="B22" s="4">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>132</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>19</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1489,19 +1472,25 @@
         <v>98</v>
       </c>
       <c r="B23" s="4">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E23" t="s">
-        <v>123</v>
+        <v>21</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1509,102 +1498,114 @@
         <v>98</v>
       </c>
       <c r="B24" s="4">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>6</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="4">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" t="s">
-        <v>126</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="A25" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="18">
+        <v>18</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="16">
-        <v>39</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>90</v>
+      <c r="A26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="4">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>128</v>
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>115</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="16">
-        <v>40</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>91</v>
+      <c r="A27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="4">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>129</v>
+        <v>46</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B28" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="E28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1613,153 +1614,110 @@
         <v>98</v>
       </c>
       <c r="B29" s="4">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="18">
-        <v>18</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21" t="s">
+      <c r="A30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="4">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B31" s="4">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="32" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="4">
-        <v>20</v>
-      </c>
-      <c r="C32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32"/>
-      <c r="J32"/>
+      <c r="A32" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="14">
+        <v>25</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="33" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="4">
-        <v>20</v>
-      </c>
-      <c r="C33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33"/>
-      <c r="J33"/>
+      <c r="A33" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="14">
+        <v>26</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="34" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="4">
-        <v>16</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" s="12"/>
-      <c r="E34" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="12"/>
-      <c r="I34"/>
-      <c r="J34" t="s">
-        <v>53</v>
+      <c r="A34" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="14">
+        <v>27</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1767,109 +1725,75 @@
         <v>98</v>
       </c>
       <c r="B35" s="4">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" s="4">
-        <v>22</v>
-      </c>
-      <c r="C36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="12"/>
-      <c r="E36" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="12"/>
-      <c r="I36"/>
-      <c r="J36"/>
+      <c r="A36" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="5">
+        <v>29</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="4">
-        <v>22</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" s="12"/>
-      <c r="E37" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="12"/>
-      <c r="I37"/>
-      <c r="J37" t="s">
-        <v>53</v>
+      <c r="A37" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="5">
+        <v>30</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="14">
-        <v>26</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15" t="s">
-        <v>143</v>
+      <c r="A38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="4">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" t="s">
+        <v>120</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="14">
-        <v>25</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15" t="s">
-        <v>143</v>
+      <c r="A39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="4">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" t="s">
+        <v>121</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1877,41 +1801,39 @@
         <v>98</v>
       </c>
       <c r="B40" s="4">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>11</v>
+        <v>122</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="18">
-        <v>24</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19" t="s">
-        <v>53</v>
+      <c r="A41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="4">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" t="s">
+        <v>123</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1919,19 +1841,19 @@
         <v>98</v>
       </c>
       <c r="B42" s="4">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>86</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="E42" t="s">
-        <v>37</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>11</v>
+        <v>124</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1939,95 +1861,109 @@
         <v>98</v>
       </c>
       <c r="B43" s="4">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>87</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="E43" t="s">
-        <v>119</v>
+        <v>125</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="14">
-        <v>27</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15" t="s">
-        <v>144</v>
+      <c r="A44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="4">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" t="s">
+        <v>126</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="5">
-        <v>11</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="A45" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="4">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E45" t="s">
+        <v>127</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" s="5">
-        <v>29</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="A46" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="16">
+        <v>39</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="5">
-        <v>30</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+      <c r="A47" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="16">
+        <v>40</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">
-    <sortState ref="A2:K47">
-      <sortCondition ref="D1"/>
+    <sortState ref="A2:J47">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed a few things about how data is updated
Moved checking of threshold change direction into spectrum class (so that it is only done once). Only create dataPlot if thresholds have changed (or not initialised).
Still more bits to change to optimise efficiency
</commit_message>
<xml_diff>
--- a/FPGA GPIO pin assignments.xlsx
+++ b/FPGA GPIO pin assignments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="168">
   <si>
     <t>Location</t>
   </si>
@@ -493,6 +493,36 @@
   </si>
   <si>
     <t>L397b</t>
+  </si>
+  <si>
+    <t>Want this to be LaserAux1</t>
+  </si>
+  <si>
+    <t>Want this to be LaserAux2</t>
+  </si>
+  <si>
+    <t>Want this to be LaserLockIn397_1</t>
+  </si>
+  <si>
+    <t>Want this to be LaserLockIn397_2</t>
+  </si>
+  <si>
+    <t>Want this to be LaserLockIn729</t>
+  </si>
+  <si>
+    <t>Want this to be LaserLockInRedSC</t>
+  </si>
+  <si>
+    <t>Want this to be MainsTrigIn</t>
+  </si>
+  <si>
+    <t>Want this to be Vout</t>
+  </si>
+  <si>
+    <t>Want this to be PMT_In_A</t>
+  </si>
+  <si>
+    <t>Want this to be PMT_In_B</t>
   </si>
 </sst>
 </file>
@@ -917,9 +947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,10 +958,11 @@
     <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" style="12" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="16" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -948,17 +979,17 @@
       <c r="D1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -977,16 +1008,16 @@
       <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1000,7 +1031,7 @@
       <c r="C3" t="s">
         <v>101</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>50</v>
       </c>
       <c r="J3" t="s">
@@ -1020,16 +1051,16 @@
       <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1046,16 +1077,16 @@
       <c r="D5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1069,7 +1100,7 @@
       <c r="C6" t="s">
         <v>104</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>51</v>
       </c>
       <c r="J6" t="s">
@@ -1087,12 +1118,12 @@
         <v>105</v>
       </c>
       <c r="D7" s="13"/>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="10"/>
       <c r="J7" s="7" t="s">
         <v>53</v>
       </c>
@@ -1110,17 +1141,17 @@
       <c r="D8" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1136,16 +1167,16 @@
       <c r="D9" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1162,16 +1193,16 @@
       <c r="D10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1188,16 +1219,16 @@
       <c r="D11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1214,16 +1245,16 @@
       <c r="D12" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="G12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="20" t="s">
         <v>7</v>
       </c>
       <c r="I12" s="19"/>
@@ -1242,16 +1273,16 @@
       <c r="D13" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="G13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="20" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="19"/>
@@ -1270,16 +1301,16 @@
       <c r="D14" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1296,16 +1327,16 @@
       <c r="D15" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1322,17 +1353,20 @@
       <c r="D16" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>7</v>
+      <c r="J16" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,17 +1382,20 @@
       <c r="D17" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>7</v>
+      <c r="H17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1385,7 +1422,7 @@
       <c r="D19" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1402,17 +1439,20 @@
       <c r="D20" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>11</v>
+      <c r="H20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1428,17 +1468,17 @@
       <c r="D21" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>11</v>
+      <c r="H21" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1454,17 +1494,20 @@
       <c r="D22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>11</v>
+      <c r="H22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1480,17 +1523,20 @@
       <c r="D23" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>11</v>
+      <c r="H23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1506,17 +1552,20 @@
       <c r="D24" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>11</v>
+      <c r="H24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1532,14 +1581,14 @@
       <c r="D25" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="20"/>
       <c r="G25" s="20"/>
-      <c r="H25" s="21" t="s">
-        <v>11</v>
-      </c>
+      <c r="H25" s="20"/>
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
     </row>
@@ -1556,11 +1605,11 @@
       <c r="D26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
         <v>115</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1576,17 +1625,17 @@
       <c r="D27" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1599,14 +1648,17 @@
       <c r="C28" t="s">
         <v>74</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1619,14 +1671,17 @@
       <c r="C29" t="s">
         <v>75</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1639,14 +1694,17 @@
       <c r="C30" t="s">
         <v>76</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="H30" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1659,14 +1717,17 @@
       <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1679,7 +1740,7 @@
       <c r="C32" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="F32" s="15" t="s">
         <v>116</v>
       </c>
       <c r="J32" s="15" t="s">
@@ -1696,7 +1757,7 @@
       <c r="C33" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="F33" s="15" t="s">
         <v>117</v>
       </c>
       <c r="J33" s="15" t="s">
@@ -1713,7 +1774,7 @@
       <c r="C34" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="F34" s="15" t="s">
         <v>118</v>
       </c>
       <c r="J34" s="15" t="s">
@@ -1730,7 +1791,7 @@
       <c r="C35" t="s">
         <v>81</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1769,11 +1830,11 @@
       <c r="D38" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
         <v>120</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1789,11 +1850,11 @@
       <c r="D39" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
         <v>121</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1809,11 +1870,11 @@
       <c r="D40" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
         <v>122</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1829,11 +1890,11 @@
       <c r="D41" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
         <v>123</v>
-      </c>
-      <c r="H41" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1849,11 +1910,11 @@
       <c r="D42" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
         <v>124</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1869,11 +1930,11 @@
       <c r="D43" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
         <v>125</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1889,11 +1950,11 @@
       <c r="D44" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
         <v>126</v>
-      </c>
-      <c r="H44" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1909,11 +1970,11 @@
       <c r="D45" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
         <v>127</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1929,14 +1990,14 @@
       <c r="D46" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E46" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
@@ -1951,14 +2012,14 @@
       <c r="D47" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="E47" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="F47" s="9"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="H47" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">

</xml_diff>

<commit_message>
Disable OK button in requestMetadata until all values are ints
</commit_message>
<xml_diff>
--- a/FPGA GPIO pin assignments.xlsx
+++ b/FPGA GPIO pin assignments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="167">
   <si>
     <t>Location</t>
   </si>
@@ -514,9 +514,6 @@
   </si>
   <si>
     <t>Want this to be MainsTrigIn</t>
-  </si>
-  <si>
-    <t>Want this to be Vout</t>
   </si>
   <si>
     <t>Want this to be PMT_In_A</t>
@@ -947,9 +944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,6 +1608,9 @@
       <c r="F26" t="s">
         <v>115</v>
       </c>
+      <c r="J26" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -1657,9 +1657,6 @@
       <c r="H28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J28" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -1681,7 +1678,7 @@
         <v>11</v>
       </c>
       <c r="J29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1703,9 +1700,6 @@
       <c r="H30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J30" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -1727,7 +1721,7 @@
         <v>11</v>
       </c>
       <c r="J31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1804,6 +1798,9 @@
       </c>
       <c r="C36" s="2" t="s">
         <v>99</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed histogram graph, added new variable to SpectroscopyViewerForm
</commit_message>
<xml_diff>
--- a/FPGA GPIO pin assignments.xlsx
+++ b/FPGA GPIO pin assignments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="169">
   <si>
     <t>Location</t>
   </si>
@@ -520,13 +520,19 @@
   </si>
   <si>
     <t>Want this to be PMT_In_B</t>
+  </si>
+  <si>
+    <t>Currently not working</t>
+  </si>
+  <si>
+    <t>No longer being used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,8 +556,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,6 +595,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -604,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -641,6 +660,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,8 +966,8 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,6 +1171,9 @@
       <c r="H8" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="J8" s="22" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1362,7 +1386,7 @@
       <c r="H16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="23" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1391,7 +1415,7 @@
       <c r="H17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="23" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1448,7 +1472,7 @@
       <c r="H20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1503,7 +1527,7 @@
       <c r="H22" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="23" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1532,7 +1556,7 @@
       <c r="H23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="23" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1561,7 +1585,7 @@
       <c r="H24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="23" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1608,7 +1632,7 @@
       <c r="F26" t="s">
         <v>115</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1637,6 +1661,9 @@
       <c r="H27" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="J27" s="23" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -1677,7 +1704,7 @@
       <c r="H29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="23" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1720,7 +1747,7 @@
       <c r="H31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="23" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pin assignments excel changed
</commit_message>
<xml_diff>
--- a/FPGA GPIO pin assignments.xlsx
+++ b/FPGA GPIO pin assignments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="170">
   <si>
     <t>Location</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>No longer being used</t>
+  </si>
+  <si>
+    <t>Want this to be Laser397_1 (needs reassigning in FPGA code)</t>
   </si>
 </sst>
 </file>
@@ -966,8 +969,8 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,6 +1686,9 @@
       </c>
       <c r="H28" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated pin assignments in FPGA. Fixed bug with graph not working properly in viewer.
Also fixed minor errors with file naming / metadata details
</commit_message>
<xml_diff>
--- a/FPGA GPIO pin assignments.xlsx
+++ b/FPGA GPIO pin assignments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="172">
   <si>
     <t>Location</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>Want this to be Laser397_1 (needs reassigning in FPGA code)</t>
+  </si>
+  <si>
+    <t>These are the new settings</t>
+  </si>
+  <si>
+    <t>These are the old, now obsolete settings</t>
   </si>
 </sst>
 </file>
@@ -966,11 +972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,10 +986,10 @@
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" style="12" customWidth="1"/>
     <col min="5" max="5" width="16" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="9" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1866,6 +1872,9 @@
       <c r="F38" t="s">
         <v>120</v>
       </c>
+      <c r="G38" s="9" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
@@ -2050,6 +2059,213 @@
       </c>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="4">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="4">
+        <v>32</v>
+      </c>
+      <c r="C50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="4">
+        <v>33</v>
+      </c>
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="4">
+        <v>34</v>
+      </c>
+      <c r="C52" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="4">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="4">
+        <v>36</v>
+      </c>
+      <c r="C54" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="4">
+        <v>37</v>
+      </c>
+      <c r="C55" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="4">
+        <v>38</v>
+      </c>
+      <c r="C56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="16">
+        <v>39</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+    </row>
+    <row r="58" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="16">
+        <v>40</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">

</xml_diff>